<commit_message>
comment demo lines in main Run Updates sample
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -48,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -416,31 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>45270.38374795145</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add code which runs if input folder path in root
on line 29

of

bibtex py

if you update root to your project

file path
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,34 +1,192 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\OneDrive\Documents\45-semester-1\module-2-Research-Methods-CS5731-PHILOSOPHY-OF-RESEARCH\5-LiteratureReview\1-proj-1\AI-Research-Project-Referencing-Program-Attempt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC9E19D-52CB-4995-A080-DE183C61595B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="4860" yWindow="1155" windowWidth="16485" windowHeight="14715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="input" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+  <si>
+    <t>Author(s) of website (year of publication) Title of webpage, available: web address [accessed date].</t>
+  </si>
+  <si>
+    <t>Author(s)</t>
+  </si>
+  <si>
+    <t>Title of webpage</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>available</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>web address</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>accessed</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>RegEx</t>
+  </si>
+  <si>
+    <t>^*.(</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x(?=))	</t>
+  </si>
+  <si>
+    <t>\)</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Italics</t>
+  </si>
+  <si>
+    <t>to string</t>
+  </si>
+  <si>
+    <t>add hyphens</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>for name in names:</t>
+  </si>
+  <si>
+    <t>if last_name:</t>
+  </si>
+  <si>
+    <t>full name</t>
+  </si>
+  <si>
+    <t>for author in authors:</t>
+  </si>
+  <si>
+    <t>encapsulation java</t>
+  </si>
+  <si>
+    <t>UL Library</t>
+  </si>
+  <si>
+    <t>https://uol.primo.exlibrisgroup.com/discovery/search?query=any,contains,encapsulation%20java&amp;tab=TAB1&amp;search_scope=MyInst_and_CI&amp;vid=353UOL_INST:353UOL_VU1&amp;lang=en&amp;offset=0</t>
+  </si>
+  <si>
+    <t>result1:</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary-wiley-com.proxy.lib.ul.ie/doi/epdf/10.1002/spe.372</t>
+  </si>
+  <si>
+    <t>JAC—Access right basedencapsulation for Java</t>
+  </si>
+  <si>
+    <t>DOI: 10.1002/spe.372</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -43,84 +201,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,19 +512,257 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C1:H19"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2">
+        <f ca="1">TODAY()</f>
+        <v>45270</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140E6F16-0257-4175-A119-1989A3531402}">
+  <dimension ref="C3:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{DFD54121-C295-4E5C-AE0E-8A07ABD8F5D4}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{E1885FF7-B4D8-41B5-AA2B-9FB3073E5C9C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E324277E-61FE-4E8B-957D-1291193836F1}">
+  <dimension ref="C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Save sample xlsx file
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,36 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\OneDrive\Documents\45-semester-1\module-2-Research-Methods-CS5731-PHILOSOPHY-OF-RESEARCH\5-LiteratureReview\1-proj-1\AI-Research-Project-Referencing-Program\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EE1738-E0D1-4B0E-97EE-D47B8EEBE86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-11610" yWindow="-21710" windowWidth="41180" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>@article{KnieselGünter2001Jrbe,</t>
+  </si>
+  <si>
+    <t>journal = {Software, practice &amp; experience},</t>
+  </si>
+  <si>
+    <t>keywords = {access rights ; aliasing ; Computer Science ; Computer Science, Software Engineering ; encapsulation ; Java ; Science &amp; Technology ; security ; Technology},</t>
+  </si>
+  <si>
+    <t>language = {eng},</t>
+  </si>
+  <si>
+    <t>number = {6},</t>
+  </si>
+  <si>
+    <t>pages = {555-576},</t>
+  </si>
+  <si>
+    <t>publisher = {John Wiley &amp; Sons, Ltd},</t>
+  </si>
+  <si>
+    <t>title = {JAC-Access right based encapsulation for Java},</t>
+  </si>
+  <si>
+    <t>volume = {31},</t>
+  </si>
+  <si>
+    <t>year = {2001},</t>
+  </si>
+  <si>
+    <t>abstract = {Unwanted effects of aliasing cause encapsulation problems in object‐oriented programming. Nevertheless, aliasing is part of common and efficient programming techniques for expressing sharing of objects and as such its general restriction is not an option in practice. This paper proposes an approach that allows full referential object sharing but adds transitive access control to object references to limit the effects of aliasing. The approach relies on well‐known properties of object‐oriented type systems but exploits them in a novel way to support an access‐right‐based model of encapsulation. It is presented as an extension of Java, called JAC (Java with Access Control). Copyright © 2001 John Wiley &amp; Sons, Ltd.},</t>
+  </si>
+  <si>
+    <t>author = {Kniesel, Günter and Theisen, Dirk},</t>
+  </si>
+  <si>
+    <t>address = {Chichester, UK},</t>
+  </si>
+  <si>
+    <t>copyright = {Copyright © 2001 John Wiley &amp; Sons, Ltd.},</t>
+  </si>
+  <si>
+    <t>issn = {0038-0644},</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,81 +108,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -411,36 +411,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>42</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>45271.02092468163</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A787DF-45D5-4C87-A784-7A8D84C74ABD}">
+  <dimension ref="C3:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>